<commit_message>
Add SCI_Int, work only just 1 time
Signed-off-by: Stanislav Prykhodko <stas@***mail***.com>
</commit_message>
<xml_diff>
--- a/SCI_Calc.xlsx
+++ b/SCI_Calc.xlsx
@@ -36,10 +36,10 @@
     <t>LSPCLK=SCI_BAUD*(BRR+1)*8</t>
   </si>
   <si>
-    <t>?SCI_BAUD?</t>
-  </si>
-  <si>
-    <t>speed</t>
+    <t>?SCI_BRR?</t>
+  </si>
+  <si>
+    <t>SCI BAUD</t>
   </si>
 </sst>
 </file>
@@ -375,7 +375,7 @@
   <dimension ref="B4:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -389,7 +389,7 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>9600</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
         <v>3</v>
@@ -400,7 +400,7 @@
         <v>2</v>
       </c>
       <c r="C5">
-        <v>162</v>
+        <v>9600</v>
       </c>
       <c r="E5" t="s">
         <v>4</v>
@@ -417,7 +417,7 @@
       </c>
       <c r="C8">
         <f>C5*(C4+1)*8</f>
-        <v>12442896</v>
+        <v>12518400</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -427,6 +427,12 @@
       <c r="C10">
         <v>115200</v>
       </c>
+      <c r="D10">
+        <v>57600</v>
+      </c>
+      <c r="E10">
+        <v>9600</v>
+      </c>
     </row>
     <row r="11" spans="2:5">
       <c r="B11" t="s">
@@ -434,7 +440,15 @@
       </c>
       <c r="C11">
         <f>C8/((C10+1)*8)</f>
-        <v>13.501289051310318</v>
+        <v>13.583215423477228</v>
+      </c>
+      <c r="D11">
+        <f>C8/((D10+1)*8)</f>
+        <v>27.166195031336262</v>
+      </c>
+      <c r="E11">
+        <f>C8/((E10+1)*8)</f>
+        <v>162.98302260181231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>